<commit_message>
adiciona documentação do projeto hroads
</commit_message>
<xml_diff>
--- a/projetoHROADS/projetohroads.xlsx
+++ b/projetoHROADS/projetohroads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2280e1d0d3b3f046/Área de Trabalho/SENAI-Sprint1-BD/projetoHROADS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77DD3928-05DD-4133-A776-2D7224051C09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{77DD3928-05DD-4133-A776-2D7224051C09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EEF57F61-9A11-4266-8B27-58F6E5A7564E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{79ABAC08-0480-4435-A639-73DA5F4693FE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Personagens</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>ClasseHabilidade</t>
-  </si>
-  <si>
-    <t>idHablidade</t>
   </si>
   <si>
     <t>Habilidades</t>
@@ -195,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -203,16 +200,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,17 +535,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263889A9-CEAD-4283-880A-12CF22D6F21A}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="5" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
     <col min="13" max="13" width="10.140625" customWidth="1"/>
     <col min="14" max="14" width="18.140625" customWidth="1"/>
@@ -552,7 +556,7 @@
     <col min="20" max="20" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,228 +566,328 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="I1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="6">
+        <v>100</v>
+      </c>
+      <c r="E3" s="6">
+        <v>80</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="7">
+        <v>43483</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="6">
+        <v>70</v>
+      </c>
+      <c r="E4" s="6">
+        <v>100</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="7">
+        <v>42446</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="6">
+        <v>75</v>
+      </c>
+      <c r="E5" s="6">
+        <v>60</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="7">
+        <v>43177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="L1" s="3" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="P1" s="4" t="s">
+      <c r="F10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>2</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6">
+        <v>2</v>
+      </c>
+      <c r="F12" s="6">
+        <v>2</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6">
+        <v>3</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="S1" s="5" t="s">
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="5"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>2</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6">
+        <v>2</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="B20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6">
         <v>3</v>
       </c>
-      <c r="L2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>10</v>
-      </c>
-      <c r="S2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3">
-        <v>80</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="6">
-        <v>43483</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>70</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="6">
-        <v>42446</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4">
-        <v>2</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4">
-        <v>2</v>
-      </c>
-      <c r="T4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5">
-        <v>75</v>
-      </c>
-      <c r="E5">
-        <v>60</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="6">
-        <v>43177</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5">
-        <v>3</v>
-      </c>
-      <c r="M5">
-        <v>3</v>
-      </c>
-      <c r="N5" t="s">
-        <v>23</v>
-      </c>
-      <c r="P5">
-        <v>3</v>
-      </c>
-      <c r="S5">
-        <v>3</v>
-      </c>
-      <c r="T5" t="s">
-        <v>25</v>
-      </c>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>